<commit_message>
adapted import to new data
</commit_message>
<xml_diff>
--- a/03 - Interactive Viz/amstat_age.xlsx
+++ b/03 - Interactive Viz/amstat_age.xlsx
@@ -344,9 +344,6 @@
     <t>5.4</t>
   </si>
   <si>
-    <t>ling_req</t>
-  </si>
-  <si>
     <t>reg</t>
   </si>
   <si>
@@ -366,6 +363,9 @@
   </si>
   <si>
     <t>empl_jobseek_c</t>
+  </si>
+  <si>
+    <t>ling_reg</t>
   </si>
 </sst>
 </file>
@@ -685,7 +685,7 @@
   <dimension ref="A1:H261"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -701,28 +701,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
         <v>105</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>106</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>111</v>
-      </c>
-      <c r="G1" t="s">
-        <v>110</v>
-      </c>
-      <c r="H1" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.15">

</xml_diff>